<commit_message>
update simulation for 5 generations.
</commit_message>
<xml_diff>
--- a/datasets/first330.xlsx
+++ b/datasets/first330.xlsx
@@ -4,10 +4,10 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="24320" windowHeight="13280"/>
+    <workbookView windowWidth="27790" windowHeight="13770"/>
   </bookViews>
   <sheets>
-    <sheet name="2024" sheetId="1" r:id="rId1"/>
+    <sheet name="2019" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -53,7 +53,7 @@
     <t>翅号</t>
   </si>
   <si>
-    <t>2018年家系号</t>
+    <t>2019年家系号</t>
   </si>
   <si>
     <t>性别</t>
@@ -2202,7 +2202,7 @@
   <dimension ref="A1:L331"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleSheetLayoutView="60" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.81818181818182" defaultRowHeight="14"/>
@@ -2259,7 +2259,7 @@
         <v>0.0202</v>
       </c>
       <c r="H2">
-        <v>2018001</v>
+        <v>2020001</v>
       </c>
       <c r="I2" t="s">
         <v>10</v>
@@ -2288,7 +2288,7 @@
         <v>0.07543</v>
       </c>
       <c r="H3">
-        <v>2018002</v>
+        <v>2020002</v>
       </c>
       <c r="I3" t="s">
         <v>10</v>
@@ -2317,7 +2317,7 @@
         <v>0.0202</v>
       </c>
       <c r="H4">
-        <v>2018003</v>
+        <v>2020003</v>
       </c>
       <c r="I4" t="s">
         <v>10</v>
@@ -2346,7 +2346,7 @@
         <v>0.05822</v>
       </c>
       <c r="H5">
-        <v>2018004</v>
+        <v>2020004</v>
       </c>
       <c r="I5" t="s">
         <v>10</v>
@@ -2375,7 +2375,7 @@
         <v>0.09592</v>
       </c>
       <c r="H6">
-        <v>2018005</v>
+        <v>2020005</v>
       </c>
       <c r="I6" t="s">
         <v>10</v>
@@ -2404,7 +2404,7 @@
         <v>0.09597</v>
       </c>
       <c r="H7">
-        <v>2018006</v>
+        <v>2020006</v>
       </c>
       <c r="I7" t="s">
         <v>10</v>
@@ -2433,7 +2433,7 @@
         <v>0.0988</v>
       </c>
       <c r="H8">
-        <v>2018007</v>
+        <v>2020007</v>
       </c>
       <c r="I8" t="s">
         <v>10</v>
@@ -2462,7 +2462,7 @@
         <v>0.10553</v>
       </c>
       <c r="H9">
-        <v>2018008</v>
+        <v>2020008</v>
       </c>
       <c r="I9" t="s">
         <v>10</v>
@@ -2491,7 +2491,7 @@
         <v>0.10049</v>
       </c>
       <c r="H10">
-        <v>2018009</v>
+        <v>2020009</v>
       </c>
       <c r="I10" t="s">
         <v>10</v>
@@ -2520,7 +2520,7 @@
         <v>0.1051</v>
       </c>
       <c r="H11">
-        <v>2018010</v>
+        <v>2020010</v>
       </c>
       <c r="I11" t="s">
         <v>10</v>
@@ -2549,7 +2549,7 @@
         <v>0.02083</v>
       </c>
       <c r="H12">
-        <v>2018011</v>
+        <v>2020011</v>
       </c>
       <c r="I12" t="s">
         <v>10</v>
@@ -2578,7 +2578,7 @@
         <v>0.00079</v>
       </c>
       <c r="H13">
-        <v>2018012</v>
+        <v>2020012</v>
       </c>
       <c r="I13" t="s">
         <v>21</v>
@@ -2607,7 +2607,7 @@
         <v>0.0183</v>
       </c>
       <c r="H14">
-        <v>2018013</v>
+        <v>2020013</v>
       </c>
       <c r="I14" t="s">
         <v>21</v>
@@ -2636,7 +2636,7 @@
         <v>0.0456</v>
       </c>
       <c r="H15">
-        <v>2018014</v>
+        <v>2020014</v>
       </c>
       <c r="I15" t="s">
         <v>21</v>
@@ -2665,7 +2665,7 @@
         <v>0.01928</v>
       </c>
       <c r="H16">
-        <v>2018015</v>
+        <v>2020015</v>
       </c>
       <c r="I16" t="s">
         <v>21</v>
@@ -2694,7 +2694,7 @@
         <v>0.01019</v>
       </c>
       <c r="H17">
-        <v>2018016</v>
+        <v>2020016</v>
       </c>
       <c r="I17" t="s">
         <v>21</v>
@@ -2723,7 +2723,7 @@
         <v>0.08926</v>
       </c>
       <c r="H18">
-        <v>2018017</v>
+        <v>2020017</v>
       </c>
       <c r="I18" t="s">
         <v>21</v>
@@ -2752,7 +2752,7 @@
         <v>0.02548</v>
       </c>
       <c r="H19">
-        <v>2018018</v>
+        <v>2020018</v>
       </c>
       <c r="I19" t="s">
         <v>21</v>
@@ -2781,7 +2781,7 @@
         <v>0.0491</v>
       </c>
       <c r="H20">
-        <v>2018019</v>
+        <v>2020019</v>
       </c>
       <c r="I20" t="s">
         <v>21</v>
@@ -2810,7 +2810,7 @@
         <v>0.02188</v>
       </c>
       <c r="H21">
-        <v>2018020</v>
+        <v>2020020</v>
       </c>
       <c r="I21" t="s">
         <v>21</v>
@@ -2839,7 +2839,7 @@
         <v>0.02407</v>
       </c>
       <c r="H22">
-        <v>2018021</v>
+        <v>2020021</v>
       </c>
       <c r="I22" t="s">
         <v>21</v>
@@ -2868,7 +2868,7 @@
         <v>0.00079</v>
       </c>
       <c r="H23">
-        <v>2018022</v>
+        <v>2020022</v>
       </c>
       <c r="I23" t="s">
         <v>21</v>
@@ -2897,7 +2897,7 @@
         <v>0.00086</v>
       </c>
       <c r="H24">
-        <v>2018023</v>
+        <v>2020023</v>
       </c>
       <c r="I24" t="s">
         <v>32</v>
@@ -2926,7 +2926,7 @@
         <v>0.04973</v>
       </c>
       <c r="H25">
-        <v>2018024</v>
+        <v>2020024</v>
       </c>
       <c r="I25" t="s">
         <v>32</v>
@@ -2955,7 +2955,7 @@
         <v>0.10507</v>
       </c>
       <c r="H26">
-        <v>2018025</v>
+        <v>2020025</v>
       </c>
       <c r="I26" t="s">
         <v>32</v>
@@ -2984,7 +2984,7 @@
         <v>0.00724</v>
       </c>
       <c r="H27">
-        <v>2018026</v>
+        <v>2020026</v>
       </c>
       <c r="I27" t="s">
         <v>32</v>
@@ -3013,7 +3013,7 @@
         <v>0.10279</v>
       </c>
       <c r="H28">
-        <v>2018027</v>
+        <v>2020027</v>
       </c>
       <c r="I28" t="s">
         <v>32</v>
@@ -3042,7 +3042,7 @@
         <v>0.10164</v>
       </c>
       <c r="H29">
-        <v>2018028</v>
+        <v>2020028</v>
       </c>
       <c r="I29" t="s">
         <v>32</v>
@@ -3071,7 +3071,7 @@
         <v>0.03138</v>
       </c>
       <c r="H30">
-        <v>2018029</v>
+        <v>2020029</v>
       </c>
       <c r="I30" t="s">
         <v>32</v>
@@ -3100,7 +3100,7 @@
         <v>0.0871</v>
       </c>
       <c r="H31">
-        <v>2018030</v>
+        <v>2020030</v>
       </c>
       <c r="I31" t="s">
         <v>32</v>
@@ -3129,7 +3129,7 @@
         <v>0.09321</v>
       </c>
       <c r="H32">
-        <v>2018031</v>
+        <v>2020031</v>
       </c>
       <c r="I32" t="s">
         <v>32</v>
@@ -3158,7 +3158,7 @@
         <v>0.09751</v>
       </c>
       <c r="H33">
-        <v>2018032</v>
+        <v>2020032</v>
       </c>
       <c r="I33" t="s">
         <v>32</v>
@@ -3187,7 +3187,7 @@
         <v>0.00086</v>
       </c>
       <c r="H34">
-        <v>2018033</v>
+        <v>2020033</v>
       </c>
       <c r="I34" t="s">
         <v>32</v>
@@ -3216,7 +3216,7 @@
         <v>0.01037</v>
       </c>
       <c r="H35">
-        <v>2018034</v>
+        <v>2020034</v>
       </c>
       <c r="I35" t="s">
         <v>43</v>
@@ -3245,7 +3245,7 @@
         <v>0.03004</v>
       </c>
       <c r="H36">
-        <v>2018035</v>
+        <v>2020035</v>
       </c>
       <c r="I36" t="s">
         <v>43</v>
@@ -3274,7 +3274,7 @@
         <v>0.10128</v>
       </c>
       <c r="H37">
-        <v>2018036</v>
+        <v>2020036</v>
       </c>
       <c r="I37" t="s">
         <v>43</v>
@@ -3303,7 +3303,7 @@
         <v>0.02034</v>
       </c>
       <c r="H38">
-        <v>2018037</v>
+        <v>2020037</v>
       </c>
       <c r="I38" t="s">
         <v>43</v>
@@ -3332,7 +3332,7 @@
         <v>0.07935</v>
       </c>
       <c r="H39">
-        <v>2018038</v>
+        <v>2020038</v>
       </c>
       <c r="I39" t="s">
         <v>43</v>
@@ -3361,7 +3361,7 @@
         <v>0.04022</v>
       </c>
       <c r="H40">
-        <v>2018039</v>
+        <v>2020039</v>
       </c>
       <c r="I40" t="s">
         <v>43</v>
@@ -3390,7 +3390,7 @@
         <v>0.01037</v>
       </c>
       <c r="H41">
-        <v>2018040</v>
+        <v>2020040</v>
       </c>
       <c r="I41" t="s">
         <v>43</v>
@@ -3419,7 +3419,7 @@
         <v>0.06067</v>
       </c>
       <c r="H42">
-        <v>2018041</v>
+        <v>2020041</v>
       </c>
       <c r="I42" t="s">
         <v>43</v>
@@ -3448,7 +3448,7 @@
         <v>0.0513</v>
       </c>
       <c r="H43">
-        <v>2018042</v>
+        <v>2020042</v>
       </c>
       <c r="I43" t="s">
         <v>43</v>
@@ -3477,7 +3477,7 @@
         <v>0.01637</v>
       </c>
       <c r="H44">
-        <v>2018043</v>
+        <v>2020043</v>
       </c>
       <c r="I44" t="s">
         <v>43</v>
@@ -3506,7 +3506,7 @@
         <v>0.06088</v>
       </c>
       <c r="H45">
-        <v>2018044</v>
+        <v>2020044</v>
       </c>
       <c r="I45" t="s">
         <v>43</v>
@@ -3535,7 +3535,7 @@
         <v>0.01271</v>
       </c>
       <c r="H46">
-        <v>2018045</v>
+        <v>2020045</v>
       </c>
       <c r="I46" t="s">
         <v>54</v>
@@ -3564,7 +3564,7 @@
         <v>0.06287</v>
       </c>
       <c r="H47">
-        <v>2018046</v>
+        <v>2020046</v>
       </c>
       <c r="I47" t="s">
         <v>54</v>
@@ -3593,7 +3593,7 @@
         <v>0.02978</v>
       </c>
       <c r="H48">
-        <v>2018047</v>
+        <v>2020047</v>
       </c>
       <c r="I48" t="s">
         <v>54</v>
@@ -3622,7 +3622,7 @@
         <v>0.08883</v>
       </c>
       <c r="H49">
-        <v>2018048</v>
+        <v>2020048</v>
       </c>
       <c r="I49" t="s">
         <v>54</v>
@@ -3651,7 +3651,7 @@
         <v>0.07194</v>
       </c>
       <c r="H50">
-        <v>2018049</v>
+        <v>2020049</v>
       </c>
       <c r="I50" t="s">
         <v>54</v>
@@ -3680,7 +3680,7 @@
         <v>0.10188</v>
       </c>
       <c r="H51">
-        <v>2018050</v>
+        <v>2020050</v>
       </c>
       <c r="I51" t="s">
         <v>54</v>
@@ -3709,7 +3709,7 @@
         <v>0.01271</v>
       </c>
       <c r="H52">
-        <v>2018051</v>
+        <v>2020051</v>
       </c>
       <c r="I52" t="s">
         <v>54</v>
@@ -3738,7 +3738,7 @@
         <v>0.09849</v>
       </c>
       <c r="H53">
-        <v>2018052</v>
+        <v>2020052</v>
       </c>
       <c r="I53" t="s">
         <v>54</v>
@@ -3767,7 +3767,7 @@
         <v>0.07262</v>
       </c>
       <c r="H54">
-        <v>2018053</v>
+        <v>2020053</v>
       </c>
       <c r="I54" t="s">
         <v>54</v>
@@ -3796,7 +3796,7 @@
         <v>0.09343</v>
       </c>
       <c r="H55">
-        <v>2018054</v>
+        <v>2020054</v>
       </c>
       <c r="I55" t="s">
         <v>54</v>
@@ -3825,7 +3825,7 @@
         <v>0.10885</v>
       </c>
       <c r="H56">
-        <v>2018055</v>
+        <v>2020055</v>
       </c>
       <c r="I56" t="s">
         <v>54</v>
@@ -3854,7 +3854,7 @@
         <v>0.01836</v>
       </c>
       <c r="H57">
-        <v>2018056</v>
+        <v>2020056</v>
       </c>
       <c r="I57" t="s">
         <v>65</v>
@@ -3883,7 +3883,7 @@
         <v>0.04438</v>
       </c>
       <c r="H58">
-        <v>2018057</v>
+        <v>2020057</v>
       </c>
       <c r="I58" t="s">
         <v>65</v>
@@ -3912,7 +3912,7 @@
         <v>0.08555</v>
       </c>
       <c r="H59">
-        <v>2018058</v>
+        <v>2020058</v>
       </c>
       <c r="I59" t="s">
         <v>65</v>
@@ -3941,7 +3941,7 @@
         <v>0.067</v>
       </c>
       <c r="H60">
-        <v>2018059</v>
+        <v>2020059</v>
       </c>
       <c r="I60" t="s">
         <v>65</v>
@@ -3970,7 +3970,7 @@
         <v>0.05359</v>
       </c>
       <c r="H61">
-        <v>2018060</v>
+        <v>2020060</v>
       </c>
       <c r="I61" t="s">
         <v>65</v>
@@ -3999,7 +3999,7 @@
         <v>0.03583</v>
       </c>
       <c r="H62">
-        <v>2018061</v>
+        <v>2020061</v>
       </c>
       <c r="I62" t="s">
         <v>65</v>
@@ -4028,7 +4028,7 @@
         <v>0.06597</v>
       </c>
       <c r="H63">
-        <v>2018062</v>
+        <v>2020062</v>
       </c>
       <c r="I63" t="s">
         <v>65</v>
@@ -4057,7 +4057,7 @@
         <v>0.06369</v>
       </c>
       <c r="H64">
-        <v>2018063</v>
+        <v>2020063</v>
       </c>
       <c r="I64" t="s">
         <v>65</v>
@@ -4086,7 +4086,7 @@
         <v>0.09582</v>
       </c>
       <c r="H65">
-        <v>2018064</v>
+        <v>2020064</v>
       </c>
       <c r="I65" t="s">
         <v>65</v>
@@ -4115,7 +4115,7 @@
         <v>0.01836</v>
       </c>
       <c r="H66">
-        <v>2018065</v>
+        <v>2020065</v>
       </c>
       <c r="I66" t="s">
         <v>65</v>
@@ -4144,7 +4144,7 @@
         <v>0.04219</v>
       </c>
       <c r="H67">
-        <v>2018066</v>
+        <v>2020066</v>
       </c>
       <c r="I67" t="s">
         <v>65</v>
@@ -4173,7 +4173,7 @@
         <v>0.00413</v>
       </c>
       <c r="H68">
-        <v>2018067</v>
+        <v>2020067</v>
       </c>
       <c r="I68" t="s">
         <v>76</v>
@@ -4202,7 +4202,7 @@
         <v>0.10814</v>
       </c>
       <c r="H69">
-        <v>2018068</v>
+        <v>2020068</v>
       </c>
       <c r="I69" t="s">
         <v>76</v>
@@ -4231,7 +4231,7 @@
         <v>0.08799</v>
       </c>
       <c r="H70">
-        <v>2018069</v>
+        <v>2020069</v>
       </c>
       <c r="I70" t="s">
         <v>76</v>
@@ -4260,7 +4260,7 @@
         <v>0.01885</v>
       </c>
       <c r="H71">
-        <v>2018070</v>
+        <v>2020070</v>
       </c>
       <c r="I71" t="s">
         <v>76</v>
@@ -4289,7 +4289,7 @@
         <v>0.0879</v>
       </c>
       <c r="H72">
-        <v>2018071</v>
+        <v>2020071</v>
       </c>
       <c r="I72" t="s">
         <v>76</v>
@@ -4318,7 +4318,7 @@
         <v>0.02498</v>
       </c>
       <c r="H73">
-        <v>2018072</v>
+        <v>2020072</v>
       </c>
       <c r="I73" t="s">
         <v>76</v>
@@ -4347,7 +4347,7 @@
         <v>0.07927</v>
       </c>
       <c r="H74">
-        <v>2018073</v>
+        <v>2020073</v>
       </c>
       <c r="I74" t="s">
         <v>76</v>
@@ -4376,7 +4376,7 @@
         <v>0.04219</v>
       </c>
       <c r="H75">
-        <v>2018074</v>
+        <v>2020074</v>
       </c>
       <c r="I75" t="s">
         <v>76</v>
@@ -4405,7 +4405,7 @@
         <v>0.00413</v>
       </c>
       <c r="H76">
-        <v>2018075</v>
+        <v>2020075</v>
       </c>
       <c r="I76" t="s">
         <v>76</v>
@@ -4434,7 +4434,7 @@
         <v>0.01362</v>
       </c>
       <c r="H77">
-        <v>2018076</v>
+        <v>2020076</v>
       </c>
       <c r="I77" t="s">
         <v>76</v>
@@ -4463,7 +4463,7 @@
         <v>0.0195</v>
       </c>
       <c r="H78">
-        <v>2018077</v>
+        <v>2020077</v>
       </c>
       <c r="I78" t="s">
         <v>76</v>
@@ -4492,7 +4492,7 @@
         <v>0.01368</v>
       </c>
       <c r="H79">
-        <v>2018078</v>
+        <v>2020078</v>
       </c>
       <c r="I79" t="s">
         <v>87</v>
@@ -4521,7 +4521,7 @@
         <v>0.10013</v>
       </c>
       <c r="H80">
-        <v>2018079</v>
+        <v>2020079</v>
       </c>
       <c r="I80" t="s">
         <v>87</v>
@@ -4550,7 +4550,7 @@
         <v>0.02743</v>
       </c>
       <c r="H81">
-        <v>2018080</v>
+        <v>2020080</v>
       </c>
       <c r="I81" t="s">
         <v>87</v>
@@ -4579,7 +4579,7 @@
         <v>0.04895</v>
       </c>
       <c r="H82">
-        <v>2018081</v>
+        <v>2020081</v>
       </c>
       <c r="I82" t="s">
         <v>87</v>
@@ -4608,7 +4608,7 @@
         <v>0.09017</v>
       </c>
       <c r="H83">
-        <v>2018082</v>
+        <v>2020082</v>
       </c>
       <c r="I83" t="s">
         <v>87</v>
@@ -4637,7 +4637,7 @@
         <v>0.03217</v>
       </c>
       <c r="H84">
-        <v>2018083</v>
+        <v>2020083</v>
       </c>
       <c r="I84" t="s">
         <v>87</v>
@@ -4666,7 +4666,7 @@
         <v>0.01499</v>
       </c>
       <c r="H85">
-        <v>2018084</v>
+        <v>2020084</v>
       </c>
       <c r="I85" t="s">
         <v>87</v>
@@ -4695,7 +4695,7 @@
         <v>0.01368</v>
       </c>
       <c r="H86">
-        <v>2018085</v>
+        <v>2020085</v>
       </c>
       <c r="I86" t="s">
         <v>87</v>
@@ -4724,7 +4724,7 @@
         <v>0.0699</v>
       </c>
       <c r="H87">
-        <v>2018086</v>
+        <v>2020086</v>
       </c>
       <c r="I87" t="s">
         <v>87</v>
@@ -4753,7 +4753,7 @@
         <v>0.0353</v>
       </c>
       <c r="H88">
-        <v>2018087</v>
+        <v>2020087</v>
       </c>
       <c r="I88" t="s">
         <v>87</v>
@@ -4782,7 +4782,7 @@
         <v>0.10913</v>
       </c>
       <c r="H89">
-        <v>2018088</v>
+        <v>2020088</v>
       </c>
       <c r="I89" t="s">
         <v>87</v>
@@ -4811,7 +4811,7 @@
         <v>0.02344</v>
       </c>
       <c r="H90">
-        <v>2018089</v>
+        <v>2020089</v>
       </c>
       <c r="I90" t="s">
         <v>98</v>
@@ -4840,7 +4840,7 @@
         <v>0.07432</v>
       </c>
       <c r="H91">
-        <v>2018090</v>
+        <v>2020090</v>
       </c>
       <c r="I91" t="s">
         <v>98</v>
@@ -4869,7 +4869,7 @@
         <v>0.08532</v>
       </c>
       <c r="H92">
-        <v>2018091</v>
+        <v>2020091</v>
       </c>
       <c r="I92" t="s">
         <v>98</v>
@@ -4898,7 +4898,7 @@
         <v>0.10057</v>
       </c>
       <c r="H93">
-        <v>2018092</v>
+        <v>2020092</v>
       </c>
       <c r="I93" t="s">
         <v>98</v>
@@ -4927,7 +4927,7 @@
         <v>0.08389</v>
       </c>
       <c r="H94">
-        <v>2018093</v>
+        <v>2020093</v>
       </c>
       <c r="I94" t="s">
         <v>98</v>
@@ -4956,7 +4956,7 @@
         <v>0.03523</v>
       </c>
       <c r="H95">
-        <v>2018094</v>
+        <v>2020094</v>
       </c>
       <c r="I95" t="s">
         <v>98</v>
@@ -4985,7 +4985,7 @@
         <v>0.02344</v>
       </c>
       <c r="H96">
-        <v>2018095</v>
+        <v>2020095</v>
       </c>
       <c r="I96" t="s">
         <v>98</v>
@@ -5014,7 +5014,7 @@
         <v>0.09869</v>
       </c>
       <c r="H97">
-        <v>2018096</v>
+        <v>2020096</v>
       </c>
       <c r="I97" t="s">
         <v>98</v>
@@ -5043,7 +5043,7 @@
         <v>0.0462</v>
       </c>
       <c r="H98">
-        <v>2018097</v>
+        <v>2020097</v>
       </c>
       <c r="I98" t="s">
         <v>98</v>
@@ -5072,7 +5072,7 @@
         <v>0.03064</v>
       </c>
       <c r="H99">
-        <v>2018098</v>
+        <v>2020098</v>
       </c>
       <c r="I99" t="s">
         <v>98</v>
@@ -5101,7 +5101,7 @@
         <v>0.06598</v>
       </c>
       <c r="H100">
-        <v>2018099</v>
+        <v>2020099</v>
       </c>
       <c r="I100" t="s">
         <v>98</v>
@@ -5130,7 +5130,7 @@
         <v>0.0303</v>
       </c>
       <c r="H101">
-        <v>2018100</v>
+        <v>2020100</v>
       </c>
       <c r="I101" t="s">
         <v>109</v>
@@ -5159,7 +5159,7 @@
         <v>0.08608</v>
       </c>
       <c r="H102">
-        <v>2018101</v>
+        <v>2020101</v>
       </c>
       <c r="I102" t="s">
         <v>109</v>
@@ -5188,7 +5188,7 @@
         <v>0.03759</v>
       </c>
       <c r="H103">
-        <v>2018102</v>
+        <v>2020102</v>
       </c>
       <c r="I103" t="s">
         <v>109</v>
@@ -5217,7 +5217,7 @@
         <v>0.03077</v>
       </c>
       <c r="H104">
-        <v>2018103</v>
+        <v>2020103</v>
       </c>
       <c r="I104" t="s">
         <v>109</v>
@@ -5246,7 +5246,7 @@
         <v>0.03616</v>
       </c>
       <c r="H105">
-        <v>2018104</v>
+        <v>2020104</v>
       </c>
       <c r="I105" t="s">
         <v>109</v>
@@ -5275,7 +5275,7 @@
         <v>0.0303</v>
       </c>
       <c r="H106">
-        <v>2018105</v>
+        <v>2020105</v>
       </c>
       <c r="I106" t="s">
         <v>109</v>
@@ -5304,7 +5304,7 @@
         <v>0.09314</v>
       </c>
       <c r="H107">
-        <v>2018106</v>
+        <v>2020106</v>
       </c>
       <c r="I107" t="s">
         <v>109</v>
@@ -5333,7 +5333,7 @@
         <v>0.06245</v>
       </c>
       <c r="H108">
-        <v>2018107</v>
+        <v>2020107</v>
       </c>
       <c r="I108" t="s">
         <v>109</v>
@@ -5362,7 +5362,7 @@
         <v>0.03078</v>
       </c>
       <c r="H109">
-        <v>2018108</v>
+        <v>2020108</v>
       </c>
       <c r="I109" t="s">
         <v>109</v>
@@ -5391,7 +5391,7 @@
         <v>0.10957</v>
       </c>
       <c r="H110">
-        <v>2018109</v>
+        <v>2020109</v>
       </c>
       <c r="I110" t="s">
         <v>109</v>
@@ -5420,7 +5420,7 @@
         <v>0.0778</v>
       </c>
       <c r="H111">
-        <v>2018110</v>
+        <v>2020110</v>
       </c>
       <c r="I111" t="s">
         <v>109</v>
@@ -5449,7 +5449,7 @@
         <v>0.0403</v>
       </c>
       <c r="H112">
-        <v>2018111</v>
+        <v>2020111</v>
       </c>
       <c r="I112" t="s">
         <v>120</v>
@@ -5478,7 +5478,7 @@
         <v>0.0139</v>
       </c>
       <c r="H113">
-        <v>2018112</v>
+        <v>2020112</v>
       </c>
       <c r="I113" t="s">
         <v>120</v>
@@ -5507,7 +5507,7 @@
         <v>0.08663</v>
       </c>
       <c r="H114">
-        <v>2018113</v>
+        <v>2020113</v>
       </c>
       <c r="I114" t="s">
         <v>120</v>
@@ -5536,7 +5536,7 @@
         <v>0.08533</v>
       </c>
       <c r="H115">
-        <v>2018114</v>
+        <v>2020114</v>
       </c>
       <c r="I115" t="s">
         <v>120</v>
@@ -5565,7 +5565,7 @@
         <v>0.07186</v>
       </c>
       <c r="H116">
-        <v>2018115</v>
+        <v>2020115</v>
       </c>
       <c r="I116" t="s">
         <v>120</v>
@@ -5594,7 +5594,7 @@
         <v>0.0597</v>
       </c>
       <c r="H117">
-        <v>2018116</v>
+        <v>2020116</v>
       </c>
       <c r="I117" t="s">
         <v>120</v>
@@ -5623,7 +5623,7 @@
         <v>0.0403</v>
       </c>
       <c r="H118">
-        <v>2018117</v>
+        <v>2020117</v>
       </c>
       <c r="I118" t="s">
         <v>120</v>
@@ -5652,7 +5652,7 @@
         <v>0.08053</v>
       </c>
       <c r="H119">
-        <v>2018118</v>
+        <v>2020118</v>
       </c>
       <c r="I119" t="s">
         <v>120</v>
@@ -5681,7 +5681,7 @@
         <v>0.08382</v>
       </c>
       <c r="H120">
-        <v>2018119</v>
+        <v>2020119</v>
       </c>
       <c r="I120" t="s">
         <v>120</v>
@@ -5710,7 +5710,7 @@
         <v>0.10695</v>
       </c>
       <c r="H121">
-        <v>2018120</v>
+        <v>2020120</v>
       </c>
       <c r="I121" t="s">
         <v>120</v>
@@ -5739,7 +5739,7 @@
         <v>0.04626</v>
       </c>
       <c r="H122">
-        <v>2018121</v>
+        <v>2020121</v>
       </c>
       <c r="I122" t="s">
         <v>120</v>
@@ -5768,7 +5768,7 @@
         <v>0.0003</v>
       </c>
       <c r="H123">
-        <v>2018122</v>
+        <v>2020122</v>
       </c>
       <c r="I123" t="s">
         <v>131</v>
@@ -5797,7 +5797,7 @@
         <v>0.03138</v>
       </c>
       <c r="H124">
-        <v>2018123</v>
+        <v>2020123</v>
       </c>
       <c r="I124" t="s">
         <v>131</v>
@@ -5826,7 +5826,7 @@
         <v>0.05156</v>
       </c>
       <c r="H125">
-        <v>2018124</v>
+        <v>2020124</v>
       </c>
       <c r="I125" t="s">
         <v>131</v>
@@ -5855,7 +5855,7 @@
         <v>0.04741</v>
       </c>
       <c r="H126">
-        <v>2018125</v>
+        <v>2020125</v>
       </c>
       <c r="I126" t="s">
         <v>131</v>
@@ -5884,7 +5884,7 @@
         <v>0.0463</v>
       </c>
       <c r="H127">
-        <v>2018126</v>
+        <v>2020126</v>
       </c>
       <c r="I127" t="s">
         <v>131</v>
@@ -5913,7 +5913,7 @@
         <v>0.04119</v>
       </c>
       <c r="H128">
-        <v>2018127</v>
+        <v>2020127</v>
       </c>
       <c r="I128" t="s">
         <v>131</v>
@@ -5942,7 +5942,7 @@
         <v>0.05548</v>
       </c>
       <c r="H129">
-        <v>2018128</v>
+        <v>2020128</v>
       </c>
       <c r="I129" t="s">
         <v>131</v>
@@ -5971,7 +5971,7 @@
         <v>0.1067</v>
       </c>
       <c r="H130">
-        <v>2018129</v>
+        <v>2020129</v>
       </c>
       <c r="I130" t="s">
         <v>131</v>
@@ -6000,7 +6000,7 @@
         <v>0.10282</v>
       </c>
       <c r="H131">
-        <v>2018130</v>
+        <v>2020130</v>
       </c>
       <c r="I131" t="s">
         <v>131</v>
@@ -6029,7 +6029,7 @@
         <v>0.0003</v>
       </c>
       <c r="H132">
-        <v>2018131</v>
+        <v>2020131</v>
       </c>
       <c r="I132" t="s">
         <v>131</v>
@@ -6058,7 +6058,7 @@
         <v>0.04295</v>
       </c>
       <c r="H133">
-        <v>2018132</v>
+        <v>2020132</v>
       </c>
       <c r="I133" t="s">
         <v>131</v>
@@ -6087,7 +6087,7 @@
         <v>0.00424</v>
       </c>
       <c r="H134">
-        <v>2018133</v>
+        <v>2020133</v>
       </c>
       <c r="I134" t="s">
         <v>142</v>
@@ -6116,7 +6116,7 @@
         <v>0.09225</v>
       </c>
       <c r="H135">
-        <v>2018134</v>
+        <v>2020134</v>
       </c>
       <c r="I135" t="s">
         <v>142</v>
@@ -6145,7 +6145,7 @@
         <v>0.05197</v>
       </c>
       <c r="H136">
-        <v>2018135</v>
+        <v>2020135</v>
       </c>
       <c r="I136" t="s">
         <v>142</v>
@@ -6174,7 +6174,7 @@
         <v>0.0923</v>
       </c>
       <c r="H137">
-        <v>2018136</v>
+        <v>2020136</v>
       </c>
       <c r="I137" t="s">
         <v>142</v>
@@ -6203,7 +6203,7 @@
         <v>0.02211</v>
       </c>
       <c r="H138">
-        <v>2018137</v>
+        <v>2020137</v>
       </c>
       <c r="I138" t="s">
         <v>142</v>
@@ -6232,7 +6232,7 @@
         <v>0.00424</v>
       </c>
       <c r="H139">
-        <v>2018138</v>
+        <v>2020138</v>
       </c>
       <c r="I139" t="s">
         <v>142</v>
@@ -6261,7 +6261,7 @@
         <v>0.02667</v>
       </c>
       <c r="H140">
-        <v>2018139</v>
+        <v>2020139</v>
       </c>
       <c r="I140" t="s">
         <v>142</v>
@@ -6290,7 +6290,7 @@
         <v>0.0242</v>
       </c>
       <c r="H141">
-        <v>2018140</v>
+        <v>2020140</v>
       </c>
       <c r="I141" t="s">
         <v>142</v>
@@ -6319,7 +6319,7 @@
         <v>0.00645</v>
       </c>
       <c r="H142">
-        <v>2018141</v>
+        <v>2020141</v>
       </c>
       <c r="I142" t="s">
         <v>142</v>
@@ -6348,7 +6348,7 @@
         <v>0.02918</v>
       </c>
       <c r="H143">
-        <v>2018142</v>
+        <v>2020142</v>
       </c>
       <c r="I143" t="s">
         <v>142</v>
@@ -6377,7 +6377,7 @@
         <v>0.09253</v>
       </c>
       <c r="H144">
-        <v>2018143</v>
+        <v>2020143</v>
       </c>
       <c r="I144" t="s">
         <v>142</v>
@@ -6406,7 +6406,7 @@
         <v>0.0218</v>
       </c>
       <c r="H145">
-        <v>2018144</v>
+        <v>2020144</v>
       </c>
       <c r="I145" t="s">
         <v>153</v>
@@ -6435,7 +6435,7 @@
         <v>0.03188</v>
       </c>
       <c r="H146">
-        <v>2018145</v>
+        <v>2020145</v>
       </c>
       <c r="I146" t="s">
         <v>153</v>
@@ -6464,7 +6464,7 @@
         <v>0.04577</v>
       </c>
       <c r="H147">
-        <v>2018146</v>
+        <v>2020146</v>
       </c>
       <c r="I147" t="s">
         <v>153</v>
@@ -6493,7 +6493,7 @@
         <v>0.0737</v>
       </c>
       <c r="H148">
-        <v>2018147</v>
+        <v>2020147</v>
       </c>
       <c r="I148" t="s">
         <v>153</v>
@@ -6522,7 +6522,7 @@
         <v>0.06022</v>
       </c>
       <c r="H149">
-        <v>2018148</v>
+        <v>2020148</v>
       </c>
       <c r="I149" t="s">
         <v>153</v>
@@ -6551,7 +6551,7 @@
         <v>0.09107</v>
       </c>
       <c r="H150">
-        <v>2018149</v>
+        <v>2020149</v>
       </c>
       <c r="I150" t="s">
         <v>153</v>
@@ -6580,7 +6580,7 @@
         <v>0.08068</v>
       </c>
       <c r="H151">
-        <v>2018150</v>
+        <v>2020150</v>
       </c>
       <c r="I151" t="s">
         <v>153</v>
@@ -6609,7 +6609,7 @@
         <v>0.02422</v>
       </c>
       <c r="H152">
-        <v>2018151</v>
+        <v>2020151</v>
       </c>
       <c r="I152" t="s">
         <v>153</v>
@@ -6638,7 +6638,7 @@
         <v>0.0218</v>
       </c>
       <c r="H153">
-        <v>2018152</v>
+        <v>2020152</v>
       </c>
       <c r="I153" t="s">
         <v>153</v>
@@ -6667,7 +6667,7 @@
         <v>0.03267</v>
       </c>
       <c r="H154">
-        <v>2018153</v>
+        <v>2020153</v>
       </c>
       <c r="I154" t="s">
         <v>153</v>
@@ -6696,7 +6696,7 @@
         <v>0.03454</v>
       </c>
       <c r="H155">
-        <v>2018154</v>
+        <v>2020154</v>
       </c>
       <c r="I155" t="s">
         <v>153</v>
@@ -6725,7 +6725,7 @@
         <v>0.01894</v>
       </c>
       <c r="H156">
-        <v>2018155</v>
+        <v>2020155</v>
       </c>
       <c r="I156" t="s">
         <v>164</v>
@@ -6754,7 +6754,7 @@
         <v>0.0641</v>
       </c>
       <c r="H157">
-        <v>2018156</v>
+        <v>2020156</v>
       </c>
       <c r="I157" t="s">
         <v>164</v>
@@ -6783,7 +6783,7 @@
         <v>0.02362</v>
       </c>
       <c r="H158">
-        <v>2018157</v>
+        <v>2020157</v>
       </c>
       <c r="I158" t="s">
         <v>164</v>
@@ -6812,7 +6812,7 @@
         <v>0.07067</v>
       </c>
       <c r="H159">
-        <v>2018158</v>
+        <v>2020158</v>
       </c>
       <c r="I159" t="s">
         <v>164</v>
@@ -6841,7 +6841,7 @@
         <v>0.01894</v>
       </c>
       <c r="H160">
-        <v>2018159</v>
+        <v>2020159</v>
       </c>
       <c r="I160" t="s">
         <v>164</v>
@@ -6870,7 +6870,7 @@
         <v>0.02755</v>
       </c>
       <c r="H161">
-        <v>2018160</v>
+        <v>2020160</v>
       </c>
       <c r="I161" t="s">
         <v>164</v>
@@ -6899,7 +6899,7 @@
         <v>0.09004</v>
       </c>
       <c r="H162">
-        <v>2018161</v>
+        <v>2020161</v>
       </c>
       <c r="I162" t="s">
         <v>164</v>
@@ -6928,7 +6928,7 @@
         <v>0.09563</v>
       </c>
       <c r="H163">
-        <v>2018162</v>
+        <v>2020162</v>
       </c>
       <c r="I163" t="s">
         <v>164</v>
@@ -6957,7 +6957,7 @@
         <v>0.07816</v>
       </c>
       <c r="H164">
-        <v>2018163</v>
+        <v>2020163</v>
       </c>
       <c r="I164" t="s">
         <v>164</v>
@@ -6986,7 +6986,7 @@
         <v>0.0966</v>
       </c>
       <c r="H165">
-        <v>2018164</v>
+        <v>2020164</v>
       </c>
       <c r="I165" t="s">
         <v>164</v>
@@ -7015,7 +7015,7 @@
         <v>0.05834</v>
       </c>
       <c r="H166">
-        <v>2018165</v>
+        <v>2020165</v>
       </c>
       <c r="I166" t="s">
         <v>164</v>
@@ -7044,7 +7044,7 @@
         <v>0.01143</v>
       </c>
       <c r="H167">
-        <v>2018166</v>
+        <v>2020166</v>
       </c>
       <c r="I167" t="s">
         <v>175</v>
@@ -7073,7 +7073,7 @@
         <v>0.05089</v>
       </c>
       <c r="H168">
-        <v>2018167</v>
+        <v>2020167</v>
       </c>
       <c r="I168" t="s">
         <v>175</v>
@@ -7102,7 +7102,7 @@
         <v>0.10805</v>
       </c>
       <c r="H169">
-        <v>2018168</v>
+        <v>2020168</v>
       </c>
       <c r="I169" t="s">
         <v>175</v>
@@ -7131,7 +7131,7 @@
         <v>0.01143</v>
       </c>
       <c r="H170">
-        <v>2018169</v>
+        <v>2020169</v>
       </c>
       <c r="I170" t="s">
         <v>175</v>
@@ -7160,7 +7160,7 @@
         <v>0.05577</v>
       </c>
       <c r="H171">
-        <v>2018170</v>
+        <v>2020170</v>
       </c>
       <c r="I171" t="s">
         <v>175</v>
@@ -7189,7 +7189,7 @@
         <v>0.10045</v>
       </c>
       <c r="H172">
-        <v>2018171</v>
+        <v>2020171</v>
       </c>
       <c r="I172" t="s">
         <v>175</v>
@@ -7218,7 +7218,7 @@
         <v>0.02805</v>
       </c>
       <c r="H173">
-        <v>2018172</v>
+        <v>2020172</v>
       </c>
       <c r="I173" t="s">
         <v>175</v>
@@ -7247,7 +7247,7 @@
         <v>0.0154</v>
       </c>
       <c r="H174">
-        <v>2018173</v>
+        <v>2020173</v>
       </c>
       <c r="I174" t="s">
         <v>175</v>
@@ -7276,7 +7276,7 @@
         <v>0.07313</v>
       </c>
       <c r="H175">
-        <v>2018174</v>
+        <v>2020174</v>
       </c>
       <c r="I175" t="s">
         <v>175</v>
@@ -7305,7 +7305,7 @@
         <v>0.08746</v>
       </c>
       <c r="H176">
-        <v>2018175</v>
+        <v>2020175</v>
       </c>
       <c r="I176" t="s">
         <v>175</v>
@@ -7334,7 +7334,7 @@
         <v>0.10975</v>
       </c>
       <c r="H177">
-        <v>2018176</v>
+        <v>2020176</v>
       </c>
       <c r="I177" t="s">
         <v>175</v>
@@ -7363,7 +7363,7 @@
         <v>0.01541</v>
       </c>
       <c r="H178">
-        <v>2018177</v>
+        <v>2020177</v>
       </c>
       <c r="I178" t="s">
         <v>186</v>
@@ -7392,7 +7392,7 @@
         <v>0.02271</v>
       </c>
       <c r="H179">
-        <v>2018178</v>
+        <v>2020178</v>
       </c>
       <c r="I179" t="s">
         <v>186</v>
@@ -7421,7 +7421,7 @@
         <v>0.01541</v>
       </c>
       <c r="H180">
-        <v>2018179</v>
+        <v>2020179</v>
       </c>
       <c r="I180" t="s">
         <v>186</v>
@@ -7450,7 +7450,7 @@
         <v>0.10686</v>
       </c>
       <c r="H181">
-        <v>2018180</v>
+        <v>2020180</v>
       </c>
       <c r="I181" t="s">
         <v>186</v>
@@ -7479,7 +7479,7 @@
         <v>0.06988</v>
       </c>
       <c r="H182">
-        <v>2018181</v>
+        <v>2020181</v>
       </c>
       <c r="I182" t="s">
         <v>186</v>
@@ -7508,7 +7508,7 @@
         <v>0.10568</v>
       </c>
       <c r="H183">
-        <v>2018182</v>
+        <v>2020182</v>
       </c>
       <c r="I183" t="s">
         <v>186</v>
@@ -7537,7 +7537,7 @@
         <v>0.08618</v>
       </c>
       <c r="H184">
-        <v>2018183</v>
+        <v>2020183</v>
       </c>
       <c r="I184" t="s">
         <v>186</v>
@@ -7566,7 +7566,7 @@
         <v>0.10048</v>
       </c>
       <c r="H185">
-        <v>2018184</v>
+        <v>2020184</v>
       </c>
       <c r="I185" t="s">
         <v>186</v>
@@ -7595,7 +7595,7 @@
         <v>0.09889</v>
       </c>
       <c r="H186">
-        <v>2018185</v>
+        <v>2020185</v>
       </c>
       <c r="I186" t="s">
         <v>186</v>
@@ -7624,7 +7624,7 @@
         <v>0.06587</v>
       </c>
       <c r="H187">
-        <v>2018186</v>
+        <v>2020186</v>
       </c>
       <c r="I187" t="s">
         <v>186</v>
@@ -7653,7 +7653,7 @@
         <v>0.03953</v>
       </c>
       <c r="H188">
-        <v>2018187</v>
+        <v>2020187</v>
       </c>
       <c r="I188" t="s">
         <v>186</v>
@@ -7682,7 +7682,7 @@
         <v>0.00187</v>
       </c>
       <c r="H189">
-        <v>2018188</v>
+        <v>2020188</v>
       </c>
       <c r="I189" t="s">
         <v>197</v>
@@ -7711,7 +7711,7 @@
         <v>0.06487</v>
       </c>
       <c r="H190">
-        <v>2018189</v>
+        <v>2020189</v>
       </c>
       <c r="I190" t="s">
         <v>197</v>
@@ -7740,7 +7740,7 @@
         <v>0.03161</v>
       </c>
       <c r="H191">
-        <v>2018190</v>
+        <v>2020190</v>
       </c>
       <c r="I191" t="s">
         <v>197</v>
@@ -7769,7 +7769,7 @@
         <v>0.02064</v>
       </c>
       <c r="H192">
-        <v>2018191</v>
+        <v>2020191</v>
       </c>
       <c r="I192" t="s">
         <v>197</v>
@@ -7798,7 +7798,7 @@
         <v>0.10021</v>
       </c>
       <c r="H193">
-        <v>2018192</v>
+        <v>2020192</v>
       </c>
       <c r="I193" t="s">
         <v>197</v>
@@ -7827,7 +7827,7 @@
         <v>0.10837</v>
       </c>
       <c r="H194">
-        <v>2018193</v>
+        <v>2020193</v>
       </c>
       <c r="I194" t="s">
         <v>197</v>
@@ -7856,7 +7856,7 @@
         <v>0.00187</v>
       </c>
       <c r="H195">
-        <v>2018194</v>
+        <v>2020194</v>
       </c>
       <c r="I195" t="s">
         <v>197</v>
@@ -7885,7 +7885,7 @@
         <v>0.03481</v>
       </c>
       <c r="H196">
-        <v>2018195</v>
+        <v>2020195</v>
       </c>
       <c r="I196" t="s">
         <v>197</v>
@@ -7914,7 +7914,7 @@
         <v>0.09686</v>
       </c>
       <c r="H197">
-        <v>2018196</v>
+        <v>2020196</v>
       </c>
       <c r="I197" t="s">
         <v>197</v>
@@ -7943,7 +7943,7 @@
         <v>0.07457</v>
       </c>
       <c r="H198">
-        <v>2018197</v>
+        <v>2020197</v>
       </c>
       <c r="I198" t="s">
         <v>197</v>
@@ -7972,7 +7972,7 @@
         <v>0.06875</v>
       </c>
       <c r="H199">
-        <v>2018198</v>
+        <v>2020198</v>
       </c>
       <c r="I199" t="s">
         <v>197</v>
@@ -8001,7 +8001,7 @@
         <v>0.00112</v>
       </c>
       <c r="H200">
-        <v>2018199</v>
+        <v>2020199</v>
       </c>
       <c r="I200" t="s">
         <v>208</v>
@@ -8030,7 +8030,7 @@
         <v>0.03687</v>
       </c>
       <c r="H201">
-        <v>2018200</v>
+        <v>2020200</v>
       </c>
       <c r="I201" t="s">
         <v>208</v>
@@ -8059,7 +8059,7 @@
         <v>0.07957</v>
       </c>
       <c r="H202">
-        <v>2018201</v>
+        <v>2020201</v>
       </c>
       <c r="I202" t="s">
         <v>208</v>
@@ -8088,7 +8088,7 @@
         <v>0.09164</v>
       </c>
       <c r="H203">
-        <v>2018202</v>
+        <v>2020202</v>
       </c>
       <c r="I203" t="s">
         <v>208</v>
@@ -8117,7 +8117,7 @@
         <v>0.04351</v>
       </c>
       <c r="H204">
-        <v>2018203</v>
+        <v>2020203</v>
       </c>
       <c r="I204" t="s">
         <v>208</v>
@@ -8146,7 +8146,7 @@
         <v>0.09515</v>
       </c>
       <c r="H205">
-        <v>2018204</v>
+        <v>2020204</v>
       </c>
       <c r="I205" t="s">
         <v>208</v>
@@ -8175,7 +8175,7 @@
         <v>0.0941</v>
       </c>
       <c r="H206">
-        <v>2018205</v>
+        <v>2020205</v>
       </c>
       <c r="I206" t="s">
         <v>208</v>
@@ -8204,7 +8204,7 @@
         <v>0.07338</v>
       </c>
       <c r="H207">
-        <v>2018206</v>
+        <v>2020206</v>
       </c>
       <c r="I207" t="s">
         <v>208</v>
@@ -8233,7 +8233,7 @@
         <v>0.00112</v>
       </c>
       <c r="H208">
-        <v>2018207</v>
+        <v>2020207</v>
       </c>
       <c r="I208" t="s">
         <v>208</v>
@@ -8262,7 +8262,7 @@
         <v>0.06285</v>
       </c>
       <c r="H209">
-        <v>2018208</v>
+        <v>2020208</v>
       </c>
       <c r="I209" t="s">
         <v>208</v>
@@ -8291,7 +8291,7 @@
         <v>0.07321</v>
       </c>
       <c r="H210">
-        <v>2018209</v>
+        <v>2020209</v>
       </c>
       <c r="I210" t="s">
         <v>208</v>
@@ -8320,7 +8320,7 @@
         <v>0.03469</v>
       </c>
       <c r="H211">
-        <v>2018210</v>
+        <v>2020210</v>
       </c>
       <c r="I211" t="s">
         <v>219</v>
@@ -8349,7 +8349,7 @@
         <v>0.04014</v>
       </c>
       <c r="H212">
-        <v>2018211</v>
+        <v>2020211</v>
       </c>
       <c r="I212" t="s">
         <v>219</v>
@@ -8378,7 +8378,7 @@
         <v>0.07367</v>
       </c>
       <c r="H213">
-        <v>2018212</v>
+        <v>2020212</v>
       </c>
       <c r="I213" t="s">
         <v>219</v>
@@ -8407,7 +8407,7 @@
         <v>0.05158</v>
       </c>
       <c r="H214">
-        <v>2018213</v>
+        <v>2020213</v>
       </c>
       <c r="I214" t="s">
         <v>219</v>
@@ -8436,7 +8436,7 @@
         <v>0.03469</v>
       </c>
       <c r="H215">
-        <v>2018214</v>
+        <v>2020214</v>
       </c>
       <c r="I215" t="s">
         <v>219</v>
@@ -8465,7 +8465,7 @@
         <v>0.05257</v>
       </c>
       <c r="H216">
-        <v>2018215</v>
+        <v>2020215</v>
       </c>
       <c r="I216" t="s">
         <v>219</v>
@@ -8494,7 +8494,7 @@
         <v>0.03698</v>
       </c>
       <c r="H217">
-        <v>2018216</v>
+        <v>2020216</v>
       </c>
       <c r="I217" t="s">
         <v>219</v>
@@ -8523,7 +8523,7 @@
         <v>0.08824</v>
       </c>
       <c r="H218">
-        <v>2018217</v>
+        <v>2020217</v>
       </c>
       <c r="I218" t="s">
         <v>219</v>
@@ -8552,7 +8552,7 @@
         <v>0.04805</v>
       </c>
       <c r="H219">
-        <v>2018218</v>
+        <v>2020218</v>
       </c>
       <c r="I219" t="s">
         <v>219</v>
@@ -8581,7 +8581,7 @@
         <v>0.07513</v>
       </c>
       <c r="H220">
-        <v>2018219</v>
+        <v>2020219</v>
       </c>
       <c r="I220" t="s">
         <v>219</v>
@@ -8610,7 +8610,7 @@
         <v>0.08705</v>
       </c>
       <c r="H221">
-        <v>2018220</v>
+        <v>2020220</v>
       </c>
       <c r="I221" t="s">
         <v>219</v>
@@ -8639,7 +8639,7 @@
         <v>0.0006</v>
       </c>
       <c r="H222">
-        <v>2018221</v>
+        <v>2020221</v>
       </c>
       <c r="I222" t="s">
         <v>230</v>
@@ -8668,7 +8668,7 @@
         <v>0.10741</v>
       </c>
       <c r="H223">
-        <v>2018222</v>
+        <v>2020222</v>
       </c>
       <c r="I223" t="s">
         <v>230</v>
@@ -8697,7 +8697,7 @@
         <v>0.0243</v>
       </c>
       <c r="H224">
-        <v>2018223</v>
+        <v>2020223</v>
       </c>
       <c r="I224" t="s">
         <v>230</v>
@@ -8726,7 +8726,7 @@
         <v>0.04507</v>
       </c>
       <c r="H225">
-        <v>2018224</v>
+        <v>2020224</v>
       </c>
       <c r="I225" t="s">
         <v>230</v>
@@ -8755,7 +8755,7 @@
         <v>0.07426</v>
       </c>
       <c r="H226">
-        <v>2018225</v>
+        <v>2020225</v>
       </c>
       <c r="I226" t="s">
         <v>230</v>
@@ -8784,7 +8784,7 @@
         <v>0.00994</v>
       </c>
       <c r="H227">
-        <v>2018226</v>
+        <v>2020226</v>
       </c>
       <c r="I227" t="s">
         <v>230</v>
@@ -8813,7 +8813,7 @@
         <v>0.02013</v>
       </c>
       <c r="H228">
-        <v>2018227</v>
+        <v>2020227</v>
       </c>
       <c r="I228" t="s">
         <v>230</v>
@@ -8842,7 +8842,7 @@
         <v>0.05855</v>
       </c>
       <c r="H229">
-        <v>2018228</v>
+        <v>2020228</v>
       </c>
       <c r="I229" t="s">
         <v>230</v>
@@ -8871,7 +8871,7 @@
         <v>0.0006</v>
       </c>
       <c r="H230">
-        <v>2018229</v>
+        <v>2020229</v>
       </c>
       <c r="I230" t="s">
         <v>230</v>
@@ -8900,7 +8900,7 @@
         <v>0.04832</v>
       </c>
       <c r="H231">
-        <v>2018230</v>
+        <v>2020230</v>
       </c>
       <c r="I231" t="s">
         <v>230</v>
@@ -8929,7 +8929,7 @@
         <v>0.1071</v>
       </c>
       <c r="H232">
-        <v>2018231</v>
+        <v>2020231</v>
       </c>
       <c r="I232" t="s">
         <v>230</v>
@@ -8958,7 +8958,7 @@
         <v>0.02327</v>
       </c>
       <c r="H233">
-        <v>2018232</v>
+        <v>2020232</v>
       </c>
       <c r="I233" t="s">
         <v>241</v>
@@ -8987,7 +8987,7 @@
         <v>0.03107</v>
       </c>
       <c r="H234">
-        <v>2018233</v>
+        <v>2020233</v>
       </c>
       <c r="I234" t="s">
         <v>241</v>
@@ -9016,7 +9016,7 @@
         <v>0.10973</v>
       </c>
       <c r="H235">
-        <v>2018234</v>
+        <v>2020234</v>
       </c>
       <c r="I235" t="s">
         <v>241</v>
@@ -9045,7 +9045,7 @@
         <v>0.0624</v>
       </c>
       <c r="H236">
-        <v>2018235</v>
+        <v>2020235</v>
       </c>
       <c r="I236" t="s">
         <v>241</v>
@@ -9074,7 +9074,7 @@
         <v>0.06927</v>
       </c>
       <c r="H237">
-        <v>2018236</v>
+        <v>2020236</v>
       </c>
       <c r="I237" t="s">
         <v>241</v>
@@ -9103,7 +9103,7 @@
         <v>0.08359</v>
       </c>
       <c r="H238">
-        <v>2018237</v>
+        <v>2020237</v>
       </c>
       <c r="I238" t="s">
         <v>241</v>
@@ -9132,7 +9132,7 @@
         <v>0.02327</v>
       </c>
       <c r="H239">
-        <v>2018238</v>
+        <v>2020238</v>
       </c>
       <c r="I239" t="s">
         <v>241</v>
@@ -9161,7 +9161,7 @@
         <v>0.07543</v>
       </c>
       <c r="H240">
-        <v>2018239</v>
+        <v>2020239</v>
       </c>
       <c r="I240" t="s">
         <v>241</v>
@@ -9190,7 +9190,7 @@
         <v>0.02705</v>
       </c>
       <c r="H241">
-        <v>2018240</v>
+        <v>2020240</v>
       </c>
       <c r="I241" t="s">
         <v>241</v>
@@ -9219,7 +9219,7 @@
         <v>0.0325</v>
       </c>
       <c r="H242">
-        <v>2018241</v>
+        <v>2020241</v>
       </c>
       <c r="I242" t="s">
         <v>241</v>
@@ -9248,7 +9248,7 @@
         <v>0.05333</v>
       </c>
       <c r="H243">
-        <v>2018242</v>
+        <v>2020242</v>
       </c>
       <c r="I243" t="s">
         <v>241</v>
@@ -9277,7 +9277,7 @@
         <v>0.00025</v>
       </c>
       <c r="H244">
-        <v>2018243</v>
+        <v>2020243</v>
       </c>
       <c r="I244" t="s">
         <v>252</v>
@@ -9306,7 +9306,7 @@
         <v>0.0594</v>
       </c>
       <c r="H245">
-        <v>2018244</v>
+        <v>2020244</v>
       </c>
       <c r="I245" t="s">
         <v>252</v>
@@ -9335,7 +9335,7 @@
         <v>0.10807</v>
       </c>
       <c r="H246">
-        <v>2018245</v>
+        <v>2020245</v>
       </c>
       <c r="I246" t="s">
         <v>252</v>
@@ -9364,7 +9364,7 @@
         <v>0.07741</v>
       </c>
       <c r="H247">
-        <v>2018246</v>
+        <v>2020246</v>
       </c>
       <c r="I247" t="s">
         <v>252</v>
@@ -9393,7 +9393,7 @@
         <v>0.06574</v>
       </c>
       <c r="H248">
-        <v>2018247</v>
+        <v>2020247</v>
       </c>
       <c r="I248" t="s">
         <v>252</v>
@@ -9422,7 +9422,7 @@
         <v>0.10524</v>
       </c>
       <c r="H249">
-        <v>2018248</v>
+        <v>2020248</v>
       </c>
       <c r="I249" t="s">
         <v>252</v>
@@ -9451,7 +9451,7 @@
         <v>0.00154</v>
       </c>
       <c r="H250">
-        <v>2018249</v>
+        <v>2020249</v>
       </c>
       <c r="I250" t="s">
         <v>252</v>
@@ -9480,7 +9480,7 @@
         <v>0.00958</v>
       </c>
       <c r="H251">
-        <v>2018250</v>
+        <v>2020250</v>
       </c>
       <c r="I251" t="s">
         <v>252</v>
@@ -9509,7 +9509,7 @@
         <v>0.02304</v>
       </c>
       <c r="H252">
-        <v>2018251</v>
+        <v>2020251</v>
       </c>
       <c r="I252" t="s">
         <v>252</v>
@@ -9538,7 +9538,7 @@
         <v>0.00025</v>
       </c>
       <c r="H253">
-        <v>2018252</v>
+        <v>2020252</v>
       </c>
       <c r="I253" t="s">
         <v>252</v>
@@ -9567,7 +9567,7 @@
         <v>0.06321</v>
       </c>
       <c r="H254">
-        <v>2018253</v>
+        <v>2020253</v>
       </c>
       <c r="I254" t="s">
         <v>252</v>
@@ -9596,7 +9596,7 @@
         <v>0.00678</v>
       </c>
       <c r="H255">
-        <v>2018254</v>
+        <v>2020254</v>
       </c>
       <c r="I255" t="s">
         <v>263</v>
@@ -9625,7 +9625,7 @@
         <v>0.03561</v>
       </c>
       <c r="H256">
-        <v>2018255</v>
+        <v>2020255</v>
       </c>
       <c r="I256" t="s">
         <v>263</v>
@@ -9654,7 +9654,7 @@
         <v>0.06738</v>
       </c>
       <c r="H257">
-        <v>2018256</v>
+        <v>2020256</v>
       </c>
       <c r="I257" t="s">
         <v>263</v>
@@ -9683,7 +9683,7 @@
         <v>0.03096</v>
       </c>
       <c r="H258">
-        <v>2018257</v>
+        <v>2020257</v>
       </c>
       <c r="I258" t="s">
         <v>263</v>
@@ -9712,7 +9712,7 @@
         <v>0.02354</v>
       </c>
       <c r="H259">
-        <v>2018258</v>
+        <v>2020258</v>
       </c>
       <c r="I259" t="s">
         <v>263</v>
@@ -9741,7 +9741,7 @@
         <v>0.06454</v>
       </c>
       <c r="H260">
-        <v>2018259</v>
+        <v>2020259</v>
       </c>
       <c r="I260" t="s">
         <v>263</v>
@@ -9770,7 +9770,7 @@
         <v>0.0543</v>
       </c>
       <c r="H261">
-        <v>2018260</v>
+        <v>2020260</v>
       </c>
       <c r="I261" t="s">
         <v>263</v>
@@ -9799,7 +9799,7 @@
         <v>0.06995</v>
       </c>
       <c r="H262">
-        <v>2018261</v>
+        <v>2020261</v>
       </c>
       <c r="I262" t="s">
         <v>263</v>
@@ -9828,7 +9828,7 @@
         <v>0.00678</v>
       </c>
       <c r="H263">
-        <v>2018262</v>
+        <v>2020262</v>
       </c>
       <c r="I263" t="s">
         <v>263</v>
@@ -9857,7 +9857,7 @@
         <v>0.00713</v>
       </c>
       <c r="H264">
-        <v>2018263</v>
+        <v>2020263</v>
       </c>
       <c r="I264" t="s">
         <v>263</v>
@@ -9886,7 +9886,7 @@
         <v>0.06983</v>
       </c>
       <c r="H265">
-        <v>2018264</v>
+        <v>2020264</v>
       </c>
       <c r="I265" t="s">
         <v>263</v>
@@ -9915,7 +9915,7 @@
         <v>0.00101</v>
       </c>
       <c r="H266">
-        <v>2018265</v>
+        <v>2020265</v>
       </c>
       <c r="I266" t="s">
         <v>274</v>
@@ -9944,7 +9944,7 @@
         <v>0.10316</v>
       </c>
       <c r="H267">
-        <v>2018266</v>
+        <v>2020266</v>
       </c>
       <c r="I267" t="s">
         <v>274</v>
@@ -9973,7 +9973,7 @@
         <v>0.06837</v>
       </c>
       <c r="H268">
-        <v>2018267</v>
+        <v>2020267</v>
       </c>
       <c r="I268" t="s">
         <v>274</v>
@@ -10002,7 +10002,7 @@
         <v>0.07226</v>
       </c>
       <c r="H269">
-        <v>2018268</v>
+        <v>2020268</v>
       </c>
       <c r="I269" t="s">
         <v>274</v>
@@ -10031,7 +10031,7 @@
         <v>0.09822</v>
       </c>
       <c r="H270">
-        <v>2018269</v>
+        <v>2020269</v>
       </c>
       <c r="I270" t="s">
         <v>274</v>
@@ -10060,7 +10060,7 @@
         <v>0.10256</v>
       </c>
       <c r="H271">
-        <v>2018270</v>
+        <v>2020270</v>
       </c>
       <c r="I271" t="s">
         <v>274</v>
@@ -10089,7 +10089,7 @@
         <v>0.05065</v>
       </c>
       <c r="H272">
-        <v>2018271</v>
+        <v>2020271</v>
       </c>
       <c r="I272" t="s">
         <v>274</v>
@@ -10118,7 +10118,7 @@
         <v>0.0873</v>
       </c>
       <c r="H273">
-        <v>2018272</v>
+        <v>2020272</v>
       </c>
       <c r="I273" t="s">
         <v>274</v>
@@ -10147,7 +10147,7 @@
         <v>0.00101</v>
       </c>
       <c r="H274">
-        <v>2018273</v>
+        <v>2020273</v>
       </c>
       <c r="I274" t="s">
         <v>274</v>
@@ -10176,7 +10176,7 @@
         <v>0.10398</v>
       </c>
       <c r="H275">
-        <v>2018274</v>
+        <v>2020274</v>
       </c>
       <c r="I275" t="s">
         <v>274</v>
@@ -10205,7 +10205,7 @@
         <v>0.09765</v>
       </c>
       <c r="H276">
-        <v>2018275</v>
+        <v>2020275</v>
       </c>
       <c r="I276" t="s">
         <v>274</v>
@@ -10234,7 +10234,7 @@
         <v>0.01115</v>
       </c>
       <c r="H277">
-        <v>2018276</v>
+        <v>2020276</v>
       </c>
       <c r="I277" t="s">
         <v>285</v>
@@ -10263,7 +10263,7 @@
         <v>0.0614</v>
       </c>
       <c r="H278">
-        <v>2018277</v>
+        <v>2020277</v>
       </c>
       <c r="I278" t="s">
         <v>285</v>
@@ -10292,7 +10292,7 @@
         <v>0.05342</v>
       </c>
       <c r="H279">
-        <v>2018278</v>
+        <v>2020278</v>
       </c>
       <c r="I279" t="s">
         <v>285</v>
@@ -10321,7 +10321,7 @@
         <v>0.01524</v>
       </c>
       <c r="H280">
-        <v>2018279</v>
+        <v>2020279</v>
       </c>
       <c r="I280" t="s">
         <v>285</v>
@@ -10350,7 +10350,7 @@
         <v>0.10876</v>
       </c>
       <c r="H281">
-        <v>2018280</v>
+        <v>2020280</v>
       </c>
       <c r="I281" t="s">
         <v>285</v>
@@ -10379,7 +10379,7 @@
         <v>0.06889</v>
       </c>
       <c r="H282">
-        <v>2018281</v>
+        <v>2020281</v>
       </c>
       <c r="I282" t="s">
         <v>285</v>
@@ -10408,7 +10408,7 @@
         <v>0.01115</v>
       </c>
       <c r="H283">
-        <v>2018282</v>
+        <v>2020282</v>
       </c>
       <c r="I283" t="s">
         <v>285</v>
@@ -10437,7 +10437,7 @@
         <v>0.03298</v>
       </c>
       <c r="H284">
-        <v>2018283</v>
+        <v>2020283</v>
       </c>
       <c r="I284" t="s">
         <v>285</v>
@@ -10466,7 +10466,7 @@
         <v>0.07002</v>
       </c>
       <c r="H285">
-        <v>2018284</v>
+        <v>2020284</v>
       </c>
       <c r="I285" t="s">
         <v>285</v>
@@ -10495,7 +10495,7 @@
         <v>0.05905</v>
       </c>
       <c r="H286">
-        <v>2018285</v>
+        <v>2020285</v>
       </c>
       <c r="I286" t="s">
         <v>285</v>
@@ -10524,7 +10524,7 @@
         <v>0.08502</v>
       </c>
       <c r="H287">
-        <v>2018286</v>
+        <v>2020286</v>
       </c>
       <c r="I287" t="s">
         <v>285</v>
@@ -10553,7 +10553,7 @@
         <v>0.00937</v>
       </c>
       <c r="H288">
-        <v>2018287</v>
+        <v>2020287</v>
       </c>
       <c r="I288" t="s">
         <v>296</v>
@@ -10582,7 +10582,7 @@
         <v>0.06843</v>
       </c>
       <c r="H289">
-        <v>2018288</v>
+        <v>2020288</v>
       </c>
       <c r="I289" t="s">
         <v>296</v>
@@ -10611,7 +10611,7 @@
         <v>0.04723</v>
       </c>
       <c r="H290">
-        <v>2018289</v>
+        <v>2020289</v>
       </c>
       <c r="I290" t="s">
         <v>296</v>
@@ -10640,7 +10640,7 @@
         <v>0.04843</v>
       </c>
       <c r="H291">
-        <v>2018290</v>
+        <v>2020290</v>
       </c>
       <c r="I291" t="s">
         <v>296</v>
@@ -10669,7 +10669,7 @@
         <v>0.00937</v>
       </c>
       <c r="H292">
-        <v>2018291</v>
+        <v>2020291</v>
       </c>
       <c r="I292" t="s">
         <v>296</v>
@@ -10698,7 +10698,7 @@
         <v>0.07955</v>
       </c>
       <c r="H293">
-        <v>2018292</v>
+        <v>2020292</v>
       </c>
       <c r="I293" t="s">
         <v>296</v>
@@ -10727,7 +10727,7 @@
         <v>0.09815</v>
       </c>
       <c r="H294">
-        <v>2018293</v>
+        <v>2020293</v>
       </c>
       <c r="I294" t="s">
         <v>296</v>
@@ -10756,7 +10756,7 @@
         <v>0.06749</v>
       </c>
       <c r="H295">
-        <v>2018294</v>
+        <v>2020294</v>
       </c>
       <c r="I295" t="s">
         <v>296</v>
@@ -10785,7 +10785,7 @@
         <v>0.07303</v>
       </c>
       <c r="H296">
-        <v>2018295</v>
+        <v>2020295</v>
       </c>
       <c r="I296" t="s">
         <v>296</v>
@@ -10814,7 +10814,7 @@
         <v>0.09744</v>
       </c>
       <c r="H297">
-        <v>2018296</v>
+        <v>2020296</v>
       </c>
       <c r="I297" t="s">
         <v>296</v>
@@ -10843,7 +10843,7 @@
         <v>0.09615</v>
       </c>
       <c r="H298">
-        <v>2018297</v>
+        <v>2020297</v>
       </c>
       <c r="I298" t="s">
         <v>296</v>
@@ -10872,7 +10872,7 @@
         <v>0.00619</v>
       </c>
       <c r="H299">
-        <v>2018298</v>
+        <v>2020298</v>
       </c>
       <c r="I299" t="s">
         <v>307</v>
@@ -10901,7 +10901,7 @@
         <v>0.03138</v>
       </c>
       <c r="H300">
-        <v>2018299</v>
+        <v>2020299</v>
       </c>
       <c r="I300" t="s">
         <v>307</v>
@@ -10930,7 +10930,7 @@
         <v>0.0615</v>
       </c>
       <c r="H301">
-        <v>2018300</v>
+        <v>2020300</v>
       </c>
       <c r="I301" t="s">
         <v>307</v>
@@ -10959,7 +10959,7 @@
         <v>0.05449</v>
       </c>
       <c r="H302">
-        <v>2018301</v>
+        <v>2020301</v>
       </c>
       <c r="I302" t="s">
         <v>307</v>
@@ -10988,7 +10988,7 @@
         <v>0.03698</v>
       </c>
       <c r="H303">
-        <v>2018302</v>
+        <v>2020302</v>
       </c>
       <c r="I303" t="s">
         <v>307</v>
@@ -11017,7 +11017,7 @@
         <v>0.09937</v>
       </c>
       <c r="H304">
-        <v>2018303</v>
+        <v>2020303</v>
       </c>
       <c r="I304" t="s">
         <v>307</v>
@@ -11046,7 +11046,7 @@
         <v>0.00619</v>
       </c>
       <c r="H305">
-        <v>2018304</v>
+        <v>2020304</v>
       </c>
       <c r="I305" t="s">
         <v>307</v>
@@ -11075,7 +11075,7 @@
         <v>0.05402</v>
       </c>
       <c r="H306">
-        <v>2018305</v>
+        <v>2020305</v>
       </c>
       <c r="I306" t="s">
         <v>307</v>
@@ -11104,7 +11104,7 @@
         <v>0.1094</v>
       </c>
       <c r="H307">
-        <v>2018306</v>
+        <v>2020306</v>
       </c>
       <c r="I307" t="s">
         <v>307</v>
@@ -11133,7 +11133,7 @@
         <v>0.03645</v>
       </c>
       <c r="H308">
-        <v>2018307</v>
+        <v>2020307</v>
       </c>
       <c r="I308" t="s">
         <v>307</v>
@@ -11162,7 +11162,7 @@
         <v>0.06275</v>
       </c>
       <c r="H309">
-        <v>2018308</v>
+        <v>2020308</v>
       </c>
       <c r="I309" t="s">
         <v>307</v>
@@ -11191,7 +11191,7 @@
         <v>0.01503</v>
       </c>
       <c r="H310">
-        <v>2018309</v>
+        <v>2020309</v>
       </c>
       <c r="I310" t="s">
         <v>318</v>
@@ -11220,7 +11220,7 @@
         <v>0.07847</v>
       </c>
       <c r="H311">
-        <v>2018310</v>
+        <v>2020310</v>
       </c>
       <c r="I311" t="s">
         <v>318</v>
@@ -11249,7 +11249,7 @@
         <v>0.01511</v>
       </c>
       <c r="H312">
-        <v>2018311</v>
+        <v>2020311</v>
       </c>
       <c r="I312" t="s">
         <v>318</v>
@@ -11278,7 +11278,7 @@
         <v>0.08439</v>
       </c>
       <c r="H313">
-        <v>2018312</v>
+        <v>2020312</v>
       </c>
       <c r="I313" t="s">
         <v>318</v>
@@ -11307,7 +11307,7 @@
         <v>0.0937</v>
       </c>
       <c r="H314">
-        <v>2018313</v>
+        <v>2020313</v>
       </c>
       <c r="I314" t="s">
         <v>318</v>
@@ -11336,7 +11336,7 @@
         <v>0.08608</v>
       </c>
       <c r="H315">
-        <v>2018314</v>
+        <v>2020314</v>
       </c>
       <c r="I315" t="s">
         <v>318</v>
@@ -11365,7 +11365,7 @@
         <v>0.0863</v>
       </c>
       <c r="H316">
-        <v>2018315</v>
+        <v>2020315</v>
       </c>
       <c r="I316" t="s">
         <v>318</v>
@@ -11394,7 +11394,7 @@
         <v>0.10722</v>
       </c>
       <c r="H317">
-        <v>2018316</v>
+        <v>2020316</v>
       </c>
       <c r="I317" t="s">
         <v>318</v>
@@ -11423,7 +11423,7 @@
         <v>0.10799</v>
       </c>
       <c r="H318">
-        <v>2018317</v>
+        <v>2020317</v>
       </c>
       <c r="I318" t="s">
         <v>318</v>
@@ -11452,7 +11452,7 @@
         <v>0.06932</v>
       </c>
       <c r="H319">
-        <v>2018318</v>
+        <v>2020318</v>
       </c>
       <c r="I319" t="s">
         <v>318</v>
@@ -11481,7 +11481,7 @@
         <v>0.01503</v>
       </c>
       <c r="H320">
-        <v>2018319</v>
+        <v>2020319</v>
       </c>
       <c r="I320" t="s">
         <v>318</v>
@@ -11510,7 +11510,7 @@
         <v>0.01602</v>
       </c>
       <c r="H321">
-        <v>2018320</v>
+        <v>2020320</v>
       </c>
       <c r="I321" t="s">
         <v>329</v>
@@ -11539,7 +11539,7 @@
         <v>0.05057</v>
       </c>
       <c r="H322">
-        <v>2018321</v>
+        <v>2020321</v>
       </c>
       <c r="I322" t="s">
         <v>329</v>
@@ -11568,7 +11568,7 @@
         <v>0.01812</v>
       </c>
       <c r="H323">
-        <v>2018322</v>
+        <v>2020322</v>
       </c>
       <c r="I323" t="s">
         <v>329</v>
@@ -11597,7 +11597,7 @@
         <v>0.01602</v>
       </c>
       <c r="H324">
-        <v>2018323</v>
+        <v>2020323</v>
       </c>
       <c r="I324" t="s">
         <v>329</v>
@@ -11626,7 +11626,7 @@
         <v>0.02166</v>
       </c>
       <c r="H325">
-        <v>2018324</v>
+        <v>2020324</v>
       </c>
       <c r="I325" t="s">
         <v>329</v>
@@ -11655,7 +11655,7 @@
         <v>0.1073</v>
       </c>
       <c r="H326">
-        <v>2018325</v>
+        <v>2020325</v>
       </c>
       <c r="I326" t="s">
         <v>329</v>
@@ -11684,7 +11684,7 @@
         <v>0.05404</v>
       </c>
       <c r="H327">
-        <v>2018326</v>
+        <v>2020326</v>
       </c>
       <c r="I327" t="s">
         <v>329</v>
@@ -11713,7 +11713,7 @@
         <v>0.05721</v>
       </c>
       <c r="H328">
-        <v>2018327</v>
+        <v>2020327</v>
       </c>
       <c r="I328" t="s">
         <v>329</v>
@@ -11742,7 +11742,7 @@
         <v>0.10526</v>
       </c>
       <c r="H329">
-        <v>2018328</v>
+        <v>2020328</v>
       </c>
       <c r="I329" t="s">
         <v>329</v>
@@ -11771,7 +11771,7 @@
         <v>0.07552</v>
       </c>
       <c r="H330">
-        <v>2018329</v>
+        <v>2020329</v>
       </c>
       <c r="I330" t="s">
         <v>329</v>
@@ -11800,7 +11800,7 @@
         <v>0.04917</v>
       </c>
       <c r="H331">
-        <v>2018330</v>
+        <v>2020330</v>
       </c>
       <c r="I331" t="s">
         <v>329</v>

</xml_diff>